<commit_message>
Corretta annotazione tra individuo di Richiesta verifica documenti e task Invio documenti per verifiche.
</commit_message>
<xml_diff>
--- a/Ontologie/Annotazioni/Annotazioniv2.xlsx
+++ b/Ontologie/Annotazioni/Annotazioniv2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fefox/Library/Mobile Documents/com~apple~CloudDocs/Università Magistrale/KEBDI/PROGETTO - Supply Chain/Ontologie/Annotazioni/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fefox/Desktop/PROGETTO - Supply Chain/Ontologie/Annotazioni/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B00A5B-7DB3-F34C-BDEF-21E92A7E3F98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3FF695-693C-6F44-B506-2D527F23B93B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="500" windowWidth="27320" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27320" yWindow="-3360" windowWidth="27320" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -566,6 +566,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{913A436B-826C-6C41-89A8-3A71A1951CD2}" name="Tabella1" displayName="Tabella1" ref="A1:D68" totalsRowShown="0">
   <autoFilter ref="A1:D68" xr:uid="{913A436B-826C-6C41-89A8-3A71A1951CD2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D68">
+    <sortCondition ref="A1:A68"/>
+  </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{4EBB2241-A739-804E-B0B4-530A46D620CF}" name="BPMNAnnotation"/>
     <tableColumn id="2" xr3:uid="{01B8A706-AA1D-C842-B094-F772202EA861}" name="AnnotationType"/>
@@ -917,8 +920,8 @@
   <sheetPr codeName="Sheet 1"/>
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -945,17 +948,17 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="D2" t="str">
         <f>VLOOKUP(A2,Foglio1!A:B,2)</f>
-        <v>Richiesta del bene</v>
+        <v>Invio fattura</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
@@ -963,17 +966,17 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="D3" t="str">
         <f>VLOOKUP(A3,Foglio1!A:B,2)</f>
-        <v>Verifica e riscontro della disponibilità del bene in magazzino</v>
+        <v>Invio fattura</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
@@ -981,17 +984,17 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="D4" t="str">
         <f>VLOOKUP(A4,Foglio1!A:B,2)</f>
-        <v>Richiesta del bene</v>
+        <v>Invio fattura</v>
       </c>
       <c r="E4" t="s">
         <v>3</v>
@@ -999,17 +1002,17 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D5" t="str">
         <f>VLOOKUP(A5,Foglio1!A:B,2)</f>
-        <v>Verifica e riscontro della disponibilità del bene in magazzino</v>
+        <v>Verifica dei documenti del bando</v>
       </c>
       <c r="E5" t="s">
         <v>3</v>
@@ -1017,17 +1020,17 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="D6" t="str">
         <f>VLOOKUP(A6,Foglio1!A:B,2)</f>
-        <v>Ripartizione del disponibile</v>
+        <v>Verifica dei documenti del bando</v>
       </c>
       <c r="E6" t="s">
         <v>3</v>
@@ -1035,17 +1038,17 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="D7" t="str">
         <f>VLOOKUP(A7,Foglio1!A:B,2)</f>
-        <v>Ripartizione del disponibile</v>
+        <v>Invio richiesta di partecipazione alla gara</v>
       </c>
       <c r="E7" t="s">
         <v>3</v>
@@ -1053,17 +1056,17 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="D8" t="str">
         <f>VLOOKUP(A8,Foglio1!A:B,2)</f>
-        <v>Allestimento picking e shipping</v>
+        <v>Invio richiesta di partecipazione alla gara</v>
       </c>
       <c r="E8" t="s">
         <v>3</v>
@@ -1071,17 +1074,17 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="D9" t="str">
         <f>VLOOKUP(A9,Foglio1!A:B,2)</f>
-        <v>Allestimento picking e shipping</v>
+        <v>Invio richiesta di partecipazione alla gara</v>
       </c>
       <c r="E9" t="s">
         <v>3</v>
@@ -1089,17 +1092,17 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="D10" t="str">
         <f>VLOOKUP(A10,Foglio1!A:B,2)</f>
-        <v>Invio del bene all'UO richiedente</v>
+        <v>Invio richiesta di partecipazione alla gara</v>
       </c>
       <c r="E10" t="s">
         <v>3</v>
@@ -1107,17 +1110,17 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="D11" t="str">
         <f>VLOOKUP(A11,Foglio1!A:B,2)</f>
-        <v>Invio del bene all'UO richiedente</v>
+        <v>Invio richiesta di partecipazione alla gara</v>
       </c>
       <c r="E11" t="s">
         <v>3</v>
@@ -1125,17 +1128,17 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="D12" t="str">
         <f>VLOOKUP(A12,Foglio1!A:B,2)</f>
-        <v>Ricezione del bene</v>
+        <v>Invio richiesta di partecipazione alla gara</v>
       </c>
       <c r="E12" t="s">
         <v>3</v>
@@ -1143,17 +1146,17 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="D13" t="str">
         <f>VLOOKUP(A13,Foglio1!A:B,2)</f>
-        <v>Ricezione del bene</v>
+        <v>Pagamento fattura</v>
       </c>
       <c r="E13" t="s">
         <v>3</v>
@@ -1161,7 +1164,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -1171,7 +1174,7 @@
       </c>
       <c r="D14" t="str">
         <f>VLOOKUP(A14,Foglio1!A:B,2)</f>
-        <v>Stoccaggio nel magazzino del reparto</v>
+        <v>Pagamento fattura</v>
       </c>
       <c r="E14" t="s">
         <v>3</v>
@@ -1179,17 +1182,17 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D15" t="str">
         <f>VLOOKUP(A15,Foglio1!A:B,2)</f>
-        <v>Stoccaggio nel magazzino del reparto</v>
+        <v>Ricezione del bene</v>
       </c>
       <c r="E15" t="s">
         <v>3</v>
@@ -1197,17 +1200,17 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D16" t="str">
         <f>VLOOKUP(A16,Foglio1!A:B,2)</f>
-        <v>Invio richiesta approvvigionamento</v>
+        <v>Ricezione del bene</v>
       </c>
       <c r="E16" t="s">
         <v>3</v>
@@ -1215,17 +1218,17 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D17" t="str">
         <f>VLOOKUP(A17,Foglio1!A:B,2)</f>
-        <v>Invio richiesta approvvigionamento</v>
+        <v>Stoccaggio nel magazzino generale</v>
       </c>
       <c r="E17" t="s">
         <v>3</v>
@@ -1233,7 +1236,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
@@ -1243,7 +1246,7 @@
       </c>
       <c r="D18" t="str">
         <f>VLOOKUP(A18,Foglio1!A:B,2)</f>
-        <v>Approvazione direzione strategica</v>
+        <v>Stoccaggio nel magazzino del reparto</v>
       </c>
       <c r="E18" t="s">
         <v>3</v>
@@ -1251,17 +1254,17 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D19" t="str">
         <f>VLOOKUP(A19,Foglio1!A:B,2)</f>
-        <v>Approvazione direzione strategica</v>
+        <v>Stoccaggio nel magazzino del reparto</v>
       </c>
       <c r="E19" t="s">
         <v>3</v>
@@ -1287,17 +1290,17 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="D21" t="str">
         <f>VLOOKUP(A21,Foglio1!A:B,2)</f>
-        <v>Verifica dei documenti del bando</v>
+        <v>Gara di appalto</v>
       </c>
       <c r="E21" t="s">
         <v>3</v>
@@ -1305,17 +1308,17 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D22" t="str">
         <f>VLOOKUP(A22,Foglio1!A:B,2)</f>
-        <v>Verifica dei documenti del bando</v>
+        <v>Gara di appalto</v>
       </c>
       <c r="E22" t="s">
         <v>3</v>
@@ -1359,17 +1362,17 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="D25" t="str">
         <f>VLOOKUP(A25,Foglio1!A:B,2)</f>
-        <v>Gara di appalto</v>
+        <v>Proclamazione vincitore concorso</v>
       </c>
       <c r="E25" t="s">
         <v>3</v>
@@ -1377,17 +1380,17 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D26" t="str">
         <f>VLOOKUP(A26,Foglio1!A:B,2)</f>
-        <v>Gara di appalto</v>
+        <v>Proclamazione vincitore concorso</v>
       </c>
       <c r="E26" t="s">
         <v>3</v>
@@ -1395,17 +1398,17 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B27" t="s">
         <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="D27" t="str">
         <f>VLOOKUP(A27,Foglio1!A:B,2)</f>
-        <v>Bando di gara</v>
+        <v>Proclamazione vincitore concorso</v>
       </c>
       <c r="E27" t="s">
         <v>3</v>
@@ -1413,17 +1416,17 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="D28" t="str">
         <f>VLOOKUP(A28,Foglio1!A:B,2)</f>
-        <v>Ricezione offerta di partecipazione</v>
+        <v>Proclamazione vincitore concorso</v>
       </c>
       <c r="E28" t="s">
         <v>3</v>
@@ -1431,17 +1434,17 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="D29" t="str">
         <f>VLOOKUP(A29,Foglio1!A:B,2)</f>
-        <v>Ricezione offerta di partecipazione</v>
+        <v>Approvazione direzione strategica</v>
       </c>
       <c r="E29" t="s">
         <v>3</v>
@@ -1449,17 +1452,17 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B30" t="s">
         <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="D30" t="str">
         <f>VLOOKUP(A30,Foglio1!A:B,2)</f>
-        <v>Ricezione offerta di partecipazione</v>
+        <v>Invio documenti per verifiche</v>
       </c>
       <c r="E30" t="s">
         <v>3</v>
@@ -1467,17 +1470,17 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="B31" t="s">
         <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="D31" t="str">
         <f>VLOOKUP(A31,Foglio1!A:B,2)</f>
-        <v>Invio richiesta di partecipazione alla gara</v>
+        <v>Invio richiesta approvvigionamento</v>
       </c>
       <c r="E31" t="s">
         <v>3</v>
@@ -1485,17 +1488,17 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C32" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="D32" t="str">
         <f>VLOOKUP(A32,Foglio1!A:B,2)</f>
-        <v>Invio richiesta di partecipazione alla gara</v>
+        <v>Invio richiesta approvvigionamento</v>
       </c>
       <c r="E32" t="s">
         <v>3</v>
@@ -1503,17 +1506,17 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="B33" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C33" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="D33" t="str">
         <f>VLOOKUP(A33,Foglio1!A:B,2)</f>
-        <v>Invio richiesta di partecipazione alla gara</v>
+        <v>Allestimento picking e shipping</v>
       </c>
       <c r="E33" t="s">
         <v>3</v>
@@ -1521,17 +1524,17 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="B34" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C34" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="D34" t="str">
         <f>VLOOKUP(A34,Foglio1!A:B,2)</f>
-        <v>Invio richiesta di partecipazione alla gara</v>
+        <v>Allestimento picking e shipping</v>
       </c>
       <c r="E34" t="s">
         <v>3</v>
@@ -1539,17 +1542,17 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D35" t="str">
         <f>VLOOKUP(A35,Foglio1!A:B,2)</f>
-        <v>Invio richiesta di partecipazione alla gara</v>
+        <v>Ricezione offerta di partecipazione</v>
       </c>
       <c r="E35" t="s">
         <v>3</v>
@@ -1557,17 +1560,17 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B36" t="s">
         <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D36" t="str">
         <f>VLOOKUP(A36,Foglio1!A:B,2)</f>
-        <v>Proclamazione vincitore concorso</v>
+        <v>Ricezione offerta di partecipazione</v>
       </c>
       <c r="E36" t="s">
         <v>3</v>
@@ -1575,17 +1578,17 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B37" t="s">
         <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D37" t="str">
         <f>VLOOKUP(A37,Foglio1!A:B,2)</f>
-        <v>Proclamazione vincitore concorso</v>
+        <v>Ricezione offerta di partecipazione</v>
       </c>
       <c r="E37" t="s">
         <v>3</v>
@@ -1593,17 +1596,17 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B38" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C38" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D38" t="str">
         <f>VLOOKUP(A38,Foglio1!A:B,2)</f>
-        <v>Proclamazione vincitore concorso</v>
+        <v>Stipula contratto</v>
       </c>
       <c r="E38" t="s">
         <v>3</v>
@@ -1611,17 +1614,17 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B39" t="s">
         <v>10</v>
       </c>
       <c r="C39" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="D39" t="str">
         <f>VLOOKUP(A39,Foglio1!A:B,2)</f>
-        <v>Proclamazione vincitore concorso</v>
+        <v>Stipula contratto</v>
       </c>
       <c r="E39" t="s">
         <v>3</v>
@@ -1635,7 +1638,7 @@
         <v>10</v>
       </c>
       <c r="C40" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="D40" t="str">
         <f>VLOOKUP(A40,Foglio1!A:B,2)</f>
@@ -1650,10 +1653,10 @@
         <v>45</v>
       </c>
       <c r="B41" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C41" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D41" t="str">
         <f>VLOOKUP(A41,Foglio1!A:B,2)</f>
@@ -1668,10 +1671,10 @@
         <v>45</v>
       </c>
       <c r="B42" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D42" t="str">
         <f>VLOOKUP(A42,Foglio1!A:B,2)</f>
@@ -1689,7 +1692,7 @@
         <v>5</v>
       </c>
       <c r="C43" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D43" t="str">
         <f>VLOOKUP(A43,Foglio1!A:B,2)</f>
@@ -1701,17 +1704,17 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="B44" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C44" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="D44" t="str">
         <f>VLOOKUP(A44,Foglio1!A:B,2)</f>
-        <v>Stipula contratto</v>
+        <v>Registrazione fattura</v>
       </c>
       <c r="E44" t="s">
         <v>3</v>
@@ -1719,17 +1722,17 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="B45" t="s">
         <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="D45" t="str">
         <f>VLOOKUP(A45,Foglio1!A:B,2)</f>
-        <v>Stipula contratto</v>
+        <v>Registrazione fattura</v>
       </c>
       <c r="E45" t="s">
         <v>3</v>
@@ -1737,17 +1740,17 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B46" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C46" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="D46" t="str">
         <f>VLOOKUP(A46,Foglio1!A:B,2)</f>
-        <v>Invio dati nuovo fornitore al magazzino</v>
+        <v>Registrazione fattura</v>
       </c>
       <c r="E46" t="s">
         <v>3</v>
@@ -1755,17 +1758,17 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B47" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C47" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="D47" t="str">
         <f>VLOOKUP(A47,Foglio1!A:B,2)</f>
-        <v>Invio dati nuovo fornitore al magazzino</v>
+        <v>Registrazione fattura</v>
       </c>
       <c r="E47" t="s">
         <v>3</v>
@@ -1773,17 +1776,17 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C48" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="D48" t="str">
         <f>VLOOKUP(A48,Foglio1!A:B,2)</f>
-        <v>Ordine di acquisto</v>
+        <v>Invio dati nuovo fornitore al magazzino</v>
       </c>
       <c r="E48" t="s">
         <v>3</v>
@@ -1791,17 +1794,17 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C49" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D49" t="str">
         <f>VLOOKUP(A49,Foglio1!A:B,2)</f>
-        <v>Ordine di acquisto</v>
+        <v>Invio dati nuovo fornitore al magazzino</v>
       </c>
       <c r="E49" t="s">
         <v>3</v>
@@ -1809,17 +1812,17 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="B50" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C50" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="D50" t="str">
         <f>VLOOKUP(A50,Foglio1!A:B,2)</f>
-        <v>Ordine di acquisto</v>
+        <v>Ripartizione del disponibile</v>
       </c>
       <c r="E50" t="s">
         <v>3</v>
@@ -1827,7 +1830,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="B51" t="s">
         <v>10</v>
@@ -1837,7 +1840,7 @@
       </c>
       <c r="D51" t="str">
         <f>VLOOKUP(A51,Foglio1!A:B,2)</f>
-        <v>Ordine di acquisto</v>
+        <v>Ripartizione del disponibile</v>
       </c>
       <c r="E51" t="s">
         <v>3</v>
@@ -1845,17 +1848,17 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="B52" t="s">
         <v>8</v>
       </c>
       <c r="C52" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D52" t="str">
         <f>VLOOKUP(A52,Foglio1!A:B,2)</f>
-        <v>Stoccaggio nel magazzino generale</v>
+        <v>Invio del bene all'UO richiedente</v>
       </c>
       <c r="E52" t="s">
         <v>3</v>
@@ -1863,7 +1866,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="B53" t="s">
         <v>10</v>
@@ -1873,7 +1876,7 @@
       </c>
       <c r="D53" t="str">
         <f>VLOOKUP(A53,Foglio1!A:B,2)</f>
-        <v>Registrazione fattura</v>
+        <v>Invio del bene all'UO richiedente</v>
       </c>
       <c r="E53" t="s">
         <v>3</v>
@@ -1881,17 +1884,17 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="B54" t="s">
         <v>5</v>
       </c>
       <c r="C54" t="s">
-        <v>57</v>
+        <v>6</v>
       </c>
       <c r="D54" t="str">
         <f>VLOOKUP(A54,Foglio1!A:B,2)</f>
-        <v>Registrazione fattura</v>
+        <v>Richiesta del bene</v>
       </c>
       <c r="E54" t="s">
         <v>3</v>
@@ -1899,17 +1902,17 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="B55" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C55" t="s">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="D55" t="str">
         <f>VLOOKUP(A55,Foglio1!A:B,2)</f>
-        <v>Registrazione fattura</v>
+        <v>Richiesta del bene</v>
       </c>
       <c r="E55" t="s">
         <v>3</v>
@@ -1917,17 +1920,17 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="B56" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C56" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="D56" t="str">
         <f>VLOOKUP(A56,Foglio1!A:B,2)</f>
-        <v>Registrazione fattura</v>
+        <v>Verifica e riscontro della disponibilità del bene in magazzino</v>
       </c>
       <c r="E56" t="s">
         <v>3</v>
@@ -1935,17 +1938,17 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>60</v>
+        <v>7</v>
       </c>
       <c r="B57" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C57" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="D57" t="str">
         <f>VLOOKUP(A57,Foglio1!A:B,2)</f>
-        <v>Pagamento fattura</v>
+        <v>Verifica e riscontro della disponibilità del bene in magazzino</v>
       </c>
       <c r="E57" t="s">
         <v>3</v>
@@ -1953,17 +1956,17 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B58" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C58" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="D58" t="str">
         <f>VLOOKUP(A58,Foglio1!A:B,2)</f>
-        <v>Pagamento fattura</v>
+        <v>Ordine di acquisto</v>
       </c>
       <c r="E58" t="s">
         <v>3</v>
@@ -1971,17 +1974,17 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="B59" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C59" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D59" t="str">
         <f>VLOOKUP(A59,Foglio1!A:B,2)</f>
-        <v>Invio richiesta di partecipazione alla gara</v>
+        <v>Ordine di acquisto</v>
       </c>
       <c r="E59" t="s">
         <v>3</v>
@@ -1989,17 +1992,17 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B60" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C60" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="D60" t="str">
         <f>VLOOKUP(A60,Foglio1!A:B,2)</f>
-        <v>Preparazione evasione ordine</v>
+        <v>Ordine di acquisto</v>
       </c>
       <c r="E60" t="s">
         <v>3</v>
@@ -2007,17 +2010,17 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="B61" t="s">
         <v>10</v>
       </c>
       <c r="C61" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="D61" t="str">
         <f>VLOOKUP(A61,Foglio1!A:B,2)</f>
-        <v>Spedizione ordine</v>
+        <v>Ordine di acquisto</v>
       </c>
       <c r="E61" t="s">
         <v>3</v>
@@ -2025,7 +2028,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B62" t="s">
         <v>10</v>
@@ -2035,7 +2038,7 @@
       </c>
       <c r="D62" t="str">
         <f>VLOOKUP(A62,Foglio1!A:B,2)</f>
-        <v>Invio fattura</v>
+        <v>Spedizione ordine</v>
       </c>
       <c r="E62" t="s">
         <v>3</v>
@@ -2043,7 +2046,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B63" t="s">
         <v>10</v>
@@ -2053,7 +2056,7 @@
       </c>
       <c r="D63" t="str">
         <f>VLOOKUP(A63,Foglio1!A:B,2)</f>
-        <v>Preparazione evasione ordine</v>
+        <v>Spedizione ordine</v>
       </c>
       <c r="E63" t="s">
         <v>3</v>
@@ -2064,10 +2067,10 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C64" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="D64" t="str">
         <f>VLOOKUP(A64,Foglio1!A:B,2)</f>
@@ -2079,17 +2082,17 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B65" t="s">
         <v>10</v>
       </c>
       <c r="C65" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D65" t="str">
         <f>VLOOKUP(A65,Foglio1!A:B,2)</f>
-        <v>Invio fattura</v>
+        <v>Preparazione evasione ordine</v>
       </c>
       <c r="E65" t="s">
         <v>3</v>
@@ -2100,10 +2103,10 @@
         <v>63</v>
       </c>
       <c r="B66" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C66" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="D66" t="str">
         <f>VLOOKUP(A66,Foglio1!A:B,2)</f>
@@ -2115,17 +2118,17 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B67" t="s">
         <v>8</v>
       </c>
       <c r="C67" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D67" t="str">
         <f>VLOOKUP(A67,Foglio1!A:B,2)</f>
-        <v>Spedizione ordine</v>
+        <v>Preparazione evasione ordine</v>
       </c>
       <c r="E67" t="s">
         <v>3</v>
@@ -2133,17 +2136,17 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="B68" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C68" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="D68" t="str">
         <f>VLOOKUP(A68,Foglio1!A:B,2)</f>
-        <v>Invio fattura</v>
+        <v>Bando di gara</v>
       </c>
       <c r="E68" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Aggiunti individui della classe Deliver_Stocked_Product. Aggiunta object properties "riguarda ordine di acquisto" con dominio Deliver_Stocked_Product e range Ordine di acquisto.
</commit_message>
<xml_diff>
--- a/Ontologie/Annotazioni/Annotazioniv2.xlsx
+++ b/Ontologie/Annotazioni/Annotazioniv2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fefox/Desktop/PROGETTO - Supply Chain/Ontologie/Annotazioni/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3FF695-693C-6F44-B506-2D527F23B93B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3EFACF8-7824-2849-9C7E-1E1D146C6BBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27320" yWindow="-3360" windowWidth="27320" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="740" yWindow="1860" windowWidth="27320" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="160">
   <si>
     <t>BPMNAnnotation</t>
   </si>
@@ -502,6 +502,15 @@
   </si>
   <si>
     <t>Fornitore</t>
+  </si>
+  <si>
+    <t>EO8199464BBC</t>
+  </si>
+  <si>
+    <t>EO8199482A97</t>
+  </si>
+  <si>
+    <t>EO81994532AB</t>
   </si>
 </sst>
 </file>
@@ -564,10 +573,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{913A436B-826C-6C41-89A8-3A71A1951CD2}" name="Tabella1" displayName="Tabella1" ref="A1:D68" totalsRowShown="0">
-  <autoFilter ref="A1:D68" xr:uid="{913A436B-826C-6C41-89A8-3A71A1951CD2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D68">
-    <sortCondition ref="A1:A68"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{913A436B-826C-6C41-89A8-3A71A1951CD2}" name="Tabella1" displayName="Tabella1" ref="A1:D71" totalsRowShown="0">
+  <autoFilter ref="A1:D71" xr:uid="{913A436B-826C-6C41-89A8-3A71A1951CD2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D71">
+    <sortCondition ref="A1:A71"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{4EBB2241-A739-804E-B0B4-530A46D620CF}" name="BPMNAnnotation"/>
@@ -918,10 +927,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet 1"/>
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2049,10 +2058,10 @@
         <v>64</v>
       </c>
       <c r="B63" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C63" t="s">
-        <v>39</v>
+        <v>159</v>
       </c>
       <c r="D63" t="str">
         <f>VLOOKUP(A63,Foglio1!A:B,2)</f>
@@ -2067,10 +2076,10 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C64" t="s">
-        <v>67</v>
+        <v>158</v>
       </c>
       <c r="D64" t="str">
         <f>VLOOKUP(A64,Foglio1!A:B,2)</f>
@@ -2082,17 +2091,17 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C65" t="s">
-        <v>40</v>
+        <v>157</v>
       </c>
       <c r="D65" t="str">
         <f>VLOOKUP(A65,Foglio1!A:B,2)</f>
-        <v>Preparazione evasione ordine</v>
+        <v>Spedizione ordine</v>
       </c>
       <c r="E65" t="s">
         <v>3</v>
@@ -2100,7 +2109,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B66" t="s">
         <v>10</v>
@@ -2110,7 +2119,7 @@
       </c>
       <c r="D66" t="str">
         <f>VLOOKUP(A66,Foglio1!A:B,2)</f>
-        <v>Preparazione evasione ordine</v>
+        <v>Spedizione ordine</v>
       </c>
       <c r="E66" t="s">
         <v>3</v>
@@ -2118,17 +2127,17 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B67" t="s">
         <v>8</v>
       </c>
       <c r="C67" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D67" t="str">
         <f>VLOOKUP(A67,Foglio1!A:B,2)</f>
-        <v>Preparazione evasione ordine</v>
+        <v>Spedizione ordine</v>
       </c>
       <c r="E67" t="s">
         <v>3</v>
@@ -2136,29 +2145,74 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="B68" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C68" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="D68" t="str">
         <f>VLOOKUP(A68,Foglio1!A:B,2)</f>
+        <v>Preparazione evasione ordine</v>
+      </c>
+      <c r="E68" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>63</v>
+      </c>
+      <c r="B69" t="s">
+        <v>10</v>
+      </c>
+      <c r="C69" t="s">
+        <v>39</v>
+      </c>
+      <c r="D69" t="str">
+        <f>VLOOKUP(A69,Foglio1!A:B,2)</f>
+        <v>Preparazione evasione ordine</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>63</v>
+      </c>
+      <c r="B70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C70" t="s">
+        <v>66</v>
+      </c>
+      <c r="D70" t="str">
+        <f>VLOOKUP(A70,Foglio1!A:B,2)</f>
+        <v>Preparazione evasione ordine</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>33</v>
+      </c>
+      <c r="B71" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71" t="s">
+        <v>28</v>
+      </c>
+      <c r="D71" t="str">
+        <f>VLOOKUP(A71,Foglio1!A:B,2)</f>
         <v>Bando di gara</v>
       </c>
-      <c r="E68" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D69" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D70" t="s">
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D72" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D73" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Apportati miglioramenti all'ontologia, tra cui l'eliminazione di annotazioni refuse.
</commit_message>
<xml_diff>
--- a/Ontologie/Annotazioni/Annotazioniv2.xlsx
+++ b/Ontologie/Annotazioni/Annotazioniv2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fefox/Desktop/PROGETTO - Supply Chain/Ontologie/Annotazioni/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3EFACF8-7824-2849-9C7E-1E1D146C6BBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD842E4-EDE2-FB40-8D58-4229E51002F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="1860" windowWidth="27320" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="172">
   <si>
     <t>BPMNAnnotation</t>
   </si>
@@ -511,6 +511,42 @@
   </si>
   <si>
     <t>EO81994532AB</t>
+  </si>
+  <si>
+    <t>OWLClass</t>
+  </si>
+  <si>
+    <t>Agente</t>
+  </si>
+  <si>
+    <t>Bando di Gara</t>
+  </si>
+  <si>
+    <t>Offerta</t>
+  </si>
+  <si>
+    <t>Organizational_Unit</t>
+  </si>
+  <si>
+    <t>Pubblicazione</t>
+  </si>
+  <si>
+    <t>Avviso Esito di Procedura</t>
+  </si>
+  <si>
+    <t>Richiesta di approvvigionamento</t>
+  </si>
+  <si>
+    <t>Contratto</t>
+  </si>
+  <si>
+    <t>Certificato di pagamento</t>
+  </si>
+  <si>
+    <t>BPMNElementLabel</t>
+  </si>
+  <si>
+    <t>BPMNElement</t>
   </si>
 </sst>
 </file>
@@ -573,16 +609,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{913A436B-826C-6C41-89A8-3A71A1951CD2}" name="Tabella1" displayName="Tabella1" ref="A1:D71" totalsRowShown="0">
-  <autoFilter ref="A1:D71" xr:uid="{913A436B-826C-6C41-89A8-3A71A1951CD2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{913A436B-826C-6C41-89A8-3A71A1951CD2}" name="Tabella1" displayName="Tabella1" ref="A1:E71" totalsRowShown="0">
+  <autoFilter ref="A1:E71" xr:uid="{913A436B-826C-6C41-89A8-3A71A1951CD2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E71">
     <sortCondition ref="A1:A71"/>
   </sortState>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{4EBB2241-A739-804E-B0B4-530A46D620CF}" name="BPMNAnnotation"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{4EBB2241-A739-804E-B0B4-530A46D620CF}" name="BPMNElement"/>
     <tableColumn id="2" xr3:uid="{01B8A706-AA1D-C842-B094-F772202EA861}" name="AnnotationType"/>
     <tableColumn id="3" xr3:uid="{662ACCCE-A4D7-1C41-85AC-694BD5FB79B1}" name="OWLElement"/>
-    <tableColumn id="5" xr3:uid="{E996A83D-F26D-A441-B0C1-3C39349589FC}" name="Etichetta" dataDxfId="0">
+    <tableColumn id="4" xr3:uid="{C08385E0-B635-B944-A2A0-B3F5ABAE3078}" name="OWLClass"/>
+    <tableColumn id="5" xr3:uid="{E996A83D-F26D-A441-B0C1-3C39349589FC}" name="BPMNElementLabel" dataDxfId="0">
       <calculatedColumnFormula>VLOOKUP(A2,Foglio1!A:B,2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -926,11 +963,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet 1"/>
-  <dimension ref="A1:E73"/>
+  <sheetPr codeName="Sheet 1">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -938,12 +977,13 @@
     <col min="1" max="1" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.83203125" customWidth="1"/>
+    <col min="5" max="5" width="51" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>171</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -952,10 +992,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+      <c r="E1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -965,15 +1008,18 @@
       <c r="C2" t="s">
         <v>40</v>
       </c>
-      <c r="D2" t="str">
+      <c r="D2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2" t="str">
         <f>VLOOKUP(A2,Foglio1!A:B,2)</f>
         <v>Invio fattura</v>
       </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>65</v>
       </c>
@@ -983,15 +1029,18 @@
       <c r="C3" t="s">
         <v>39</v>
       </c>
-      <c r="D3" t="str">
+      <c r="D3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E3" t="str">
         <f>VLOOKUP(A3,Foglio1!A:B,2)</f>
         <v>Invio fattura</v>
       </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>65</v>
       </c>
@@ -1001,15 +1050,18 @@
       <c r="C4" t="s">
         <v>50</v>
       </c>
-      <c r="D4" t="str">
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" t="str">
         <f>VLOOKUP(A4,Foglio1!A:B,2)</f>
         <v>Invio fattura</v>
       </c>
-      <c r="E4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1019,15 +1071,18 @@
       <c r="C5" t="s">
         <v>27</v>
       </c>
-      <c r="D5" t="str">
+      <c r="D5" t="s">
+        <v>161</v>
+      </c>
+      <c r="E5" t="str">
         <f>VLOOKUP(A5,Foglio1!A:B,2)</f>
         <v>Verifica dei documenti del bando</v>
       </c>
-      <c r="E5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1037,15 +1092,18 @@
       <c r="C6" t="s">
         <v>28</v>
       </c>
-      <c r="D6" t="str">
+      <c r="D6" t="s">
+        <v>162</v>
+      </c>
+      <c r="E6" t="str">
         <f>VLOOKUP(A6,Foglio1!A:B,2)</f>
         <v>Verifica dei documenti del bando</v>
       </c>
-      <c r="E6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -1055,15 +1113,18 @@
       <c r="C7" t="s">
         <v>35</v>
       </c>
-      <c r="D7" t="str">
+      <c r="D7" t="s">
+        <v>163</v>
+      </c>
+      <c r="E7" t="str">
         <f>VLOOKUP(A7,Foglio1!A:B,2)</f>
         <v>Invio richiesta di partecipazione alla gara</v>
       </c>
-      <c r="E7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1073,15 +1134,18 @@
       <c r="C8" t="s">
         <v>36</v>
       </c>
-      <c r="D8" t="str">
+      <c r="D8" t="s">
+        <v>163</v>
+      </c>
+      <c r="E8" t="str">
         <f>VLOOKUP(A8,Foglio1!A:B,2)</f>
         <v>Invio richiesta di partecipazione alla gara</v>
       </c>
-      <c r="E8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -1091,15 +1155,18 @@
       <c r="C9" t="s">
         <v>37</v>
       </c>
-      <c r="D9" t="str">
+      <c r="D9" t="s">
+        <v>163</v>
+      </c>
+      <c r="E9" t="str">
         <f>VLOOKUP(A9,Foglio1!A:B,2)</f>
         <v>Invio richiesta di partecipazione alla gara</v>
       </c>
-      <c r="E9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -1109,15 +1176,18 @@
       <c r="C10" t="s">
         <v>39</v>
       </c>
-      <c r="D10" t="str">
+      <c r="D10" t="s">
+        <v>161</v>
+      </c>
+      <c r="E10" t="str">
         <f>VLOOKUP(A10,Foglio1!A:B,2)</f>
         <v>Invio richiesta di partecipazione alla gara</v>
       </c>
-      <c r="E10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -1127,15 +1197,18 @@
       <c r="C11" t="s">
         <v>40</v>
       </c>
-      <c r="D11" t="str">
+      <c r="D11" t="s">
+        <v>161</v>
+      </c>
+      <c r="E11" t="str">
         <f>VLOOKUP(A11,Foglio1!A:B,2)</f>
         <v>Invio richiesta di partecipazione alla gara</v>
       </c>
-      <c r="E11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -1145,15 +1218,18 @@
       <c r="C12" t="s">
         <v>62</v>
       </c>
-      <c r="D12" t="str">
+      <c r="D12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" t="str">
         <f>VLOOKUP(A12,Foglio1!A:B,2)</f>
         <v>Invio richiesta di partecipazione alla gara</v>
       </c>
-      <c r="E12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -1163,15 +1239,18 @@
       <c r="C13" t="s">
         <v>61</v>
       </c>
-      <c r="D13" t="str">
+      <c r="D13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" t="str">
         <f>VLOOKUP(A13,Foglio1!A:B,2)</f>
         <v>Pagamento fattura</v>
       </c>
-      <c r="E13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -1181,15 +1260,18 @@
       <c r="C14" t="s">
         <v>11</v>
       </c>
-      <c r="D14" t="str">
+      <c r="D14" t="s">
+        <v>164</v>
+      </c>
+      <c r="E14" t="str">
         <f>VLOOKUP(A14,Foglio1!A:B,2)</f>
         <v>Pagamento fattura</v>
       </c>
-      <c r="E14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1199,15 +1281,18 @@
       <c r="C15" t="s">
         <v>11</v>
       </c>
-      <c r="D15" t="str">
+      <c r="D15" t="s">
+        <v>164</v>
+      </c>
+      <c r="E15" t="str">
         <f>VLOOKUP(A15,Foglio1!A:B,2)</f>
         <v>Ricezione del bene</v>
       </c>
-      <c r="E15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1217,15 +1302,18 @@
       <c r="C16" t="s">
         <v>19</v>
       </c>
-      <c r="D16" t="str">
+      <c r="D16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" t="str">
         <f>VLOOKUP(A16,Foglio1!A:B,2)</f>
         <v>Ricezione del bene</v>
       </c>
-      <c r="E16" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -1235,15 +1323,18 @@
       <c r="C17" t="s">
         <v>21</v>
       </c>
-      <c r="D17" t="str">
+      <c r="D17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" t="str">
         <f>VLOOKUP(A17,Foglio1!A:B,2)</f>
         <v>Stoccaggio nel magazzino generale</v>
       </c>
-      <c r="E17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1253,15 +1344,18 @@
       <c r="C18" t="s">
         <v>11</v>
       </c>
-      <c r="D18" t="str">
+      <c r="D18" t="s">
+        <v>164</v>
+      </c>
+      <c r="E18" t="str">
         <f>VLOOKUP(A18,Foglio1!A:B,2)</f>
         <v>Stoccaggio nel magazzino del reparto</v>
       </c>
-      <c r="E18" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1271,15 +1365,18 @@
       <c r="C19" t="s">
         <v>21</v>
       </c>
-      <c r="D19" t="str">
+      <c r="D19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" t="str">
         <f>VLOOKUP(A19,Foglio1!A:B,2)</f>
         <v>Stoccaggio nel magazzino del reparto</v>
       </c>
-      <c r="E19" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1289,15 +1386,18 @@
       <c r="C20" t="s">
         <v>11</v>
       </c>
-      <c r="D20" t="str">
+      <c r="D20" t="s">
+        <v>164</v>
+      </c>
+      <c r="E20" t="str">
         <f>VLOOKUP(A20,Foglio1!A:B,2)</f>
         <v>Invio documenti per verifiche</v>
       </c>
-      <c r="E20" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1307,15 +1407,18 @@
       <c r="C21" t="s">
         <v>11</v>
       </c>
-      <c r="D21" t="str">
+      <c r="D21" t="s">
+        <v>164</v>
+      </c>
+      <c r="E21" t="str">
         <f>VLOOKUP(A21,Foglio1!A:B,2)</f>
         <v>Gara di appalto</v>
       </c>
-      <c r="E21" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -1325,15 +1428,18 @@
       <c r="C22" t="s">
         <v>32</v>
       </c>
-      <c r="D22" t="str">
+      <c r="D22" t="s">
+        <v>165</v>
+      </c>
+      <c r="E22" t="str">
         <f>VLOOKUP(A22,Foglio1!A:B,2)</f>
         <v>Gara di appalto</v>
       </c>
-      <c r="E22" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1343,15 +1449,18 @@
       <c r="C23" t="s">
         <v>30</v>
       </c>
-      <c r="D23" t="str">
+      <c r="D23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" t="str">
         <f>VLOOKUP(A23,Foglio1!A:B,2)</f>
         <v>Rettifica documenti</v>
       </c>
-      <c r="E23" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1361,15 +1470,18 @@
       <c r="C24" t="s">
         <v>11</v>
       </c>
-      <c r="D24" t="str">
+      <c r="D24" t="s">
+        <v>164</v>
+      </c>
+      <c r="E24" t="str">
         <f>VLOOKUP(A24,Foglio1!A:B,2)</f>
         <v>Rettifica documenti</v>
       </c>
-      <c r="E24" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -1379,15 +1491,18 @@
       <c r="C25" t="s">
         <v>42</v>
       </c>
-      <c r="D25" t="str">
+      <c r="D25" t="s">
+        <v>166</v>
+      </c>
+      <c r="E25" t="str">
         <f>VLOOKUP(A25,Foglio1!A:B,2)</f>
         <v>Proclamazione vincitore concorso</v>
       </c>
-      <c r="E25" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -1397,15 +1512,18 @@
       <c r="C26" t="s">
         <v>43</v>
       </c>
-      <c r="D26" t="str">
+      <c r="D26" t="s">
+        <v>166</v>
+      </c>
+      <c r="E26" t="str">
         <f>VLOOKUP(A26,Foglio1!A:B,2)</f>
         <v>Proclamazione vincitore concorso</v>
       </c>
-      <c r="E26" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -1415,15 +1533,18 @@
       <c r="C27" t="s">
         <v>44</v>
       </c>
-      <c r="D27" t="str">
+      <c r="D27" t="s">
+        <v>166</v>
+      </c>
+      <c r="E27" t="str">
         <f>VLOOKUP(A27,Foglio1!A:B,2)</f>
         <v>Proclamazione vincitore concorso</v>
       </c>
-      <c r="E27" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -1433,15 +1554,18 @@
       <c r="C28" t="s">
         <v>11</v>
       </c>
-      <c r="D28" t="str">
+      <c r="D28" t="s">
+        <v>164</v>
+      </c>
+      <c r="E28" t="str">
         <f>VLOOKUP(A28,Foglio1!A:B,2)</f>
         <v>Proclamazione vincitore concorso</v>
       </c>
-      <c r="E28" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -1451,15 +1575,18 @@
       <c r="C29" t="s">
         <v>11</v>
       </c>
-      <c r="D29" t="str">
+      <c r="D29" t="s">
+        <v>164</v>
+      </c>
+      <c r="E29" t="str">
         <f>VLOOKUP(A29,Foglio1!A:B,2)</f>
         <v>Approvazione direzione strategica</v>
       </c>
-      <c r="E29" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>25</v>
       </c>
@@ -1469,15 +1596,18 @@
       <c r="C30" t="s">
         <v>24</v>
       </c>
-      <c r="D30" t="str">
+      <c r="D30" t="s">
+        <v>112</v>
+      </c>
+      <c r="E30" t="str">
         <f>VLOOKUP(A30,Foglio1!A:B,2)</f>
         <v>Invio documenti per verifiche</v>
       </c>
-      <c r="E30" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -1487,15 +1617,18 @@
       <c r="C31" t="s">
         <v>6</v>
       </c>
-      <c r="D31" t="str">
+      <c r="D31" t="s">
+        <v>167</v>
+      </c>
+      <c r="E31" t="str">
         <f>VLOOKUP(A31,Foglio1!A:B,2)</f>
         <v>Invio richiesta approvvigionamento</v>
       </c>
-      <c r="E31" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -1505,15 +1638,18 @@
       <c r="C32" t="s">
         <v>11</v>
       </c>
-      <c r="D32" t="str">
+      <c r="D32" t="s">
+        <v>164</v>
+      </c>
+      <c r="E32" t="str">
         <f>VLOOKUP(A32,Foglio1!A:B,2)</f>
         <v>Invio richiesta approvvigionamento</v>
       </c>
-      <c r="E32" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -1523,15 +1659,18 @@
       <c r="C33" t="s">
         <v>11</v>
       </c>
-      <c r="D33" t="str">
+      <c r="D33" t="s">
+        <v>164</v>
+      </c>
+      <c r="E33" t="str">
         <f>VLOOKUP(A33,Foglio1!A:B,2)</f>
         <v>Allestimento picking e shipping</v>
       </c>
-      <c r="E33" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -1541,15 +1680,18 @@
       <c r="C34" t="s">
         <v>15</v>
       </c>
-      <c r="D34" t="str">
+      <c r="D34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" t="str">
         <f>VLOOKUP(A34,Foglio1!A:B,2)</f>
         <v>Allestimento picking e shipping</v>
       </c>
-      <c r="E34" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1559,15 +1701,18 @@
       <c r="C35" t="s">
         <v>35</v>
       </c>
-      <c r="D35" t="str">
+      <c r="D35" t="s">
+        <v>163</v>
+      </c>
+      <c r="E35" t="str">
         <f>VLOOKUP(A35,Foglio1!A:B,2)</f>
         <v>Ricezione offerta di partecipazione</v>
       </c>
-      <c r="E35" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1577,15 +1722,18 @@
       <c r="C36" t="s">
         <v>36</v>
       </c>
-      <c r="D36" t="str">
+      <c r="D36" t="s">
+        <v>163</v>
+      </c>
+      <c r="E36" t="str">
         <f>VLOOKUP(A36,Foglio1!A:B,2)</f>
         <v>Ricezione offerta di partecipazione</v>
       </c>
-      <c r="E36" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -1595,15 +1743,18 @@
       <c r="C37" t="s">
         <v>37</v>
       </c>
-      <c r="D37" t="str">
+      <c r="D37" t="s">
+        <v>163</v>
+      </c>
+      <c r="E37" t="str">
         <f>VLOOKUP(A37,Foglio1!A:B,2)</f>
         <v>Ricezione offerta di partecipazione</v>
       </c>
-      <c r="E37" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>45</v>
       </c>
@@ -1613,15 +1764,18 @@
       <c r="C38" t="s">
         <v>11</v>
       </c>
-      <c r="D38" t="str">
+      <c r="D38" t="s">
+        <v>164</v>
+      </c>
+      <c r="E38" t="str">
         <f>VLOOKUP(A38,Foglio1!A:B,2)</f>
         <v>Stipula contratto</v>
       </c>
-      <c r="E38" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -1631,15 +1785,18 @@
       <c r="C39" t="s">
         <v>39</v>
       </c>
-      <c r="D39" t="str">
+      <c r="D39" t="s">
+        <v>161</v>
+      </c>
+      <c r="E39" t="str">
         <f>VLOOKUP(A39,Foglio1!A:B,2)</f>
         <v>Stipula contratto</v>
       </c>
-      <c r="E39" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -1649,15 +1806,18 @@
       <c r="C40" t="s">
         <v>40</v>
       </c>
-      <c r="D40" t="str">
+      <c r="D40" t="s">
+        <v>161</v>
+      </c>
+      <c r="E40" t="str">
         <f>VLOOKUP(A40,Foglio1!A:B,2)</f>
         <v>Stipula contratto</v>
       </c>
-      <c r="E40" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -1667,15 +1827,18 @@
       <c r="C41" t="s">
         <v>46</v>
       </c>
-      <c r="D41" t="str">
+      <c r="D41" t="s">
+        <v>168</v>
+      </c>
+      <c r="E41" t="str">
         <f>VLOOKUP(A41,Foglio1!A:B,2)</f>
         <v>Stipula contratto</v>
       </c>
-      <c r="E41" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -1685,15 +1848,18 @@
       <c r="C42" t="s">
         <v>47</v>
       </c>
-      <c r="D42" t="str">
+      <c r="D42" t="s">
+        <v>168</v>
+      </c>
+      <c r="E42" t="str">
         <f>VLOOKUP(A42,Foglio1!A:B,2)</f>
         <v>Stipula contratto</v>
       </c>
-      <c r="E42" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -1703,15 +1869,18 @@
       <c r="C43" t="s">
         <v>48</v>
       </c>
-      <c r="D43" t="str">
+      <c r="D43" t="s">
+        <v>168</v>
+      </c>
+      <c r="E43" t="str">
         <f>VLOOKUP(A43,Foglio1!A:B,2)</f>
         <v>Stipula contratto</v>
       </c>
-      <c r="E43" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>56</v>
       </c>
@@ -1721,15 +1890,18 @@
       <c r="C44" t="s">
         <v>11</v>
       </c>
-      <c r="D44" t="str">
+      <c r="D44" t="s">
+        <v>164</v>
+      </c>
+      <c r="E44" t="str">
         <f>VLOOKUP(A44,Foglio1!A:B,2)</f>
         <v>Registrazione fattura</v>
       </c>
-      <c r="E44" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>56</v>
       </c>
@@ -1739,15 +1911,18 @@
       <c r="C45" t="s">
         <v>57</v>
       </c>
-      <c r="D45" t="str">
+      <c r="D45" t="s">
+        <v>169</v>
+      </c>
+      <c r="E45" t="str">
         <f>VLOOKUP(A45,Foglio1!A:B,2)</f>
         <v>Registrazione fattura</v>
       </c>
-      <c r="E45" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>56</v>
       </c>
@@ -1757,15 +1932,18 @@
       <c r="C46" t="s">
         <v>58</v>
       </c>
-      <c r="D46" t="str">
+      <c r="D46" t="s">
+        <v>169</v>
+      </c>
+      <c r="E46" t="str">
         <f>VLOOKUP(A46,Foglio1!A:B,2)</f>
         <v>Registrazione fattura</v>
       </c>
-      <c r="E46" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>56</v>
       </c>
@@ -1775,15 +1953,18 @@
       <c r="C47" t="s">
         <v>59</v>
       </c>
-      <c r="D47" t="str">
+      <c r="D47" t="s">
+        <v>169</v>
+      </c>
+      <c r="E47" t="str">
         <f>VLOOKUP(A47,Foglio1!A:B,2)</f>
         <v>Registrazione fattura</v>
       </c>
-      <c r="E47" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>49</v>
       </c>
@@ -1793,15 +1974,18 @@
       <c r="C48" t="s">
         <v>11</v>
       </c>
-      <c r="D48" t="str">
+      <c r="D48" t="s">
+        <v>164</v>
+      </c>
+      <c r="E48" t="str">
         <f>VLOOKUP(A48,Foglio1!A:B,2)</f>
         <v>Invio dati nuovo fornitore al magazzino</v>
       </c>
-      <c r="E48" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -1811,15 +1995,18 @@
       <c r="C49" t="s">
         <v>50</v>
       </c>
-      <c r="D49" t="str">
+      <c r="D49" t="s">
+        <v>50</v>
+      </c>
+      <c r="E49" t="str">
         <f>VLOOKUP(A49,Foglio1!A:B,2)</f>
         <v>Invio dati nuovo fornitore al magazzino</v>
       </c>
-      <c r="E49" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>12</v>
       </c>
@@ -1829,15 +2016,18 @@
       <c r="C50" t="s">
         <v>13</v>
       </c>
-      <c r="D50" t="str">
+      <c r="D50" t="s">
+        <v>13</v>
+      </c>
+      <c r="E50" t="str">
         <f>VLOOKUP(A50,Foglio1!A:B,2)</f>
         <v>Ripartizione del disponibile</v>
       </c>
-      <c r="E50" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>12</v>
       </c>
@@ -1847,15 +2037,18 @@
       <c r="C51" t="s">
         <v>11</v>
       </c>
-      <c r="D51" t="str">
+      <c r="D51" t="s">
+        <v>164</v>
+      </c>
+      <c r="E51" t="str">
         <f>VLOOKUP(A51,Foglio1!A:B,2)</f>
         <v>Ripartizione del disponibile</v>
       </c>
-      <c r="E51" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>16</v>
       </c>
@@ -1865,15 +2058,18 @@
       <c r="C52" t="s">
         <v>17</v>
       </c>
-      <c r="D52" t="str">
+      <c r="D52" t="s">
+        <v>17</v>
+      </c>
+      <c r="E52" t="str">
         <f>VLOOKUP(A52,Foglio1!A:B,2)</f>
         <v>Invio del bene all'UO richiedente</v>
       </c>
-      <c r="E52" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>16</v>
       </c>
@@ -1883,15 +2079,18 @@
       <c r="C53" t="s">
         <v>11</v>
       </c>
-      <c r="D53" t="str">
+      <c r="D53" t="s">
+        <v>164</v>
+      </c>
+      <c r="E53" t="str">
         <f>VLOOKUP(A53,Foglio1!A:B,2)</f>
         <v>Invio del bene all'UO richiedente</v>
       </c>
-      <c r="E53" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>4</v>
       </c>
@@ -1901,15 +2100,18 @@
       <c r="C54" t="s">
         <v>6</v>
       </c>
-      <c r="D54" t="str">
+      <c r="D54" t="s">
+        <v>167</v>
+      </c>
+      <c r="E54" t="str">
         <f>VLOOKUP(A54,Foglio1!A:B,2)</f>
         <v>Richiesta del bene</v>
       </c>
-      <c r="E54" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>4</v>
       </c>
@@ -1919,15 +2121,18 @@
       <c r="C55" t="s">
         <v>11</v>
       </c>
-      <c r="D55" t="str">
+      <c r="D55" t="s">
+        <v>164</v>
+      </c>
+      <c r="E55" t="str">
         <f>VLOOKUP(A55,Foglio1!A:B,2)</f>
         <v>Richiesta del bene</v>
       </c>
-      <c r="E55" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F55" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>7</v>
       </c>
@@ -1937,15 +2142,18 @@
       <c r="C56" t="s">
         <v>9</v>
       </c>
-      <c r="D56" t="str">
+      <c r="D56" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" t="str">
         <f>VLOOKUP(A56,Foglio1!A:B,2)</f>
         <v>Verifica e riscontro della disponibilità del bene in magazzino</v>
       </c>
-      <c r="E56" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>7</v>
       </c>
@@ -1955,15 +2163,18 @@
       <c r="C57" t="s">
         <v>11</v>
       </c>
-      <c r="D57" t="str">
+      <c r="D57" t="s">
+        <v>164</v>
+      </c>
+      <c r="E57" t="str">
         <f>VLOOKUP(A57,Foglio1!A:B,2)</f>
         <v>Verifica e riscontro della disponibilità del bene in magazzino</v>
       </c>
-      <c r="E57" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F57" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>51</v>
       </c>
@@ -1973,15 +2184,18 @@
       <c r="C58" t="s">
         <v>52</v>
       </c>
-      <c r="D58" t="str">
+      <c r="D58" t="s">
+        <v>136</v>
+      </c>
+      <c r="E58" t="str">
         <f>VLOOKUP(A58,Foglio1!A:B,2)</f>
         <v>Ordine di acquisto</v>
       </c>
-      <c r="E58" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F58" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>51</v>
       </c>
@@ -1991,15 +2205,18 @@
       <c r="C59" t="s">
         <v>53</v>
       </c>
-      <c r="D59" t="str">
+      <c r="D59" t="s">
+        <v>136</v>
+      </c>
+      <c r="E59" t="str">
         <f>VLOOKUP(A59,Foglio1!A:B,2)</f>
         <v>Ordine di acquisto</v>
       </c>
-      <c r="E59" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>51</v>
       </c>
@@ -2009,15 +2226,18 @@
       <c r="C60" t="s">
         <v>54</v>
       </c>
-      <c r="D60" t="str">
+      <c r="D60" t="s">
+        <v>136</v>
+      </c>
+      <c r="E60" t="str">
         <f>VLOOKUP(A60,Foglio1!A:B,2)</f>
         <v>Ordine di acquisto</v>
       </c>
-      <c r="E60" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F60" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>51</v>
       </c>
@@ -2027,15 +2247,18 @@
       <c r="C61" t="s">
         <v>11</v>
       </c>
-      <c r="D61" t="str">
+      <c r="D61" t="s">
+        <v>164</v>
+      </c>
+      <c r="E61" t="str">
         <f>VLOOKUP(A61,Foglio1!A:B,2)</f>
         <v>Ordine di acquisto</v>
       </c>
-      <c r="E61" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>64</v>
       </c>
@@ -2045,15 +2268,18 @@
       <c r="C62" t="s">
         <v>40</v>
       </c>
-      <c r="D62" t="str">
+      <c r="D62" t="s">
+        <v>161</v>
+      </c>
+      <c r="E62" t="str">
         <f>VLOOKUP(A62,Foglio1!A:B,2)</f>
         <v>Spedizione ordine</v>
       </c>
-      <c r="E62" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F62" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>64</v>
       </c>
@@ -2063,15 +2289,18 @@
       <c r="C63" t="s">
         <v>159</v>
       </c>
-      <c r="D63" t="str">
+      <c r="D63" t="s">
+        <v>67</v>
+      </c>
+      <c r="E63" t="str">
         <f>VLOOKUP(A63,Foglio1!A:B,2)</f>
         <v>Spedizione ordine</v>
       </c>
-      <c r="E63" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>64</v>
       </c>
@@ -2081,15 +2310,18 @@
       <c r="C64" t="s">
         <v>158</v>
       </c>
-      <c r="D64" t="str">
+      <c r="D64" t="s">
+        <v>67</v>
+      </c>
+      <c r="E64" t="str">
         <f>VLOOKUP(A64,Foglio1!A:B,2)</f>
         <v>Spedizione ordine</v>
       </c>
-      <c r="E64" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F64" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -2099,15 +2331,18 @@
       <c r="C65" t="s">
         <v>157</v>
       </c>
-      <c r="D65" t="str">
+      <c r="D65" t="s">
+        <v>67</v>
+      </c>
+      <c r="E65" t="str">
         <f>VLOOKUP(A65,Foglio1!A:B,2)</f>
         <v>Spedizione ordine</v>
       </c>
-      <c r="E65" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F65" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -2117,15 +2352,18 @@
       <c r="C66" t="s">
         <v>39</v>
       </c>
-      <c r="D66" t="str">
+      <c r="D66" t="s">
+        <v>161</v>
+      </c>
+      <c r="E66" t="str">
         <f>VLOOKUP(A66,Foglio1!A:B,2)</f>
         <v>Spedizione ordine</v>
       </c>
-      <c r="E66" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F66" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>64</v>
       </c>
@@ -2135,15 +2373,18 @@
       <c r="C67" t="s">
         <v>67</v>
       </c>
-      <c r="D67" t="str">
+      <c r="D67" t="s">
+        <v>67</v>
+      </c>
+      <c r="E67" t="str">
         <f>VLOOKUP(A67,Foglio1!A:B,2)</f>
         <v>Spedizione ordine</v>
       </c>
-      <c r="E67" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F67" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>63</v>
       </c>
@@ -2153,15 +2394,18 @@
       <c r="C68" t="s">
         <v>40</v>
       </c>
-      <c r="D68" t="str">
+      <c r="D68" t="s">
+        <v>161</v>
+      </c>
+      <c r="E68" t="str">
         <f>VLOOKUP(A68,Foglio1!A:B,2)</f>
         <v>Preparazione evasione ordine</v>
       </c>
-      <c r="E68" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F68" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>63</v>
       </c>
@@ -2171,12 +2415,15 @@
       <c r="C69" t="s">
         <v>39</v>
       </c>
-      <c r="D69" t="str">
+      <c r="D69" t="s">
+        <v>161</v>
+      </c>
+      <c r="E69" t="str">
         <f>VLOOKUP(A69,Foglio1!A:B,2)</f>
         <v>Preparazione evasione ordine</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>63</v>
       </c>
@@ -2186,12 +2433,15 @@
       <c r="C70" t="s">
         <v>66</v>
       </c>
-      <c r="D70" t="str">
+      <c r="D70" t="s">
+        <v>66</v>
+      </c>
+      <c r="E70" t="str">
         <f>VLOOKUP(A70,Foglio1!A:B,2)</f>
         <v>Preparazione evasione ordine</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>33</v>
       </c>
@@ -2201,24 +2451,28 @@
       <c r="C71" t="s">
         <v>28</v>
       </c>
-      <c r="D71" t="str">
+      <c r="D71" t="s">
+        <v>162</v>
+      </c>
+      <c r="E71" t="str">
         <f>VLOOKUP(A71,Foglio1!A:B,2)</f>
         <v>Bando di gara</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D72" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D73" t="s">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E72" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E73" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="55" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -2713,6 +2967,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>